<commit_message>
updated stresstest excel file
</commit_message>
<xml_diff>
--- a/test/CVaS.PerfTests/stresstest.xlsx
+++ b/test/CVaS.PerfTests/stresstest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7365" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="38">
   <si>
     <t>Latency</t>
   </si>
@@ -86,9 +86,6 @@
     <t>StdDev</t>
   </si>
   <si>
-    <t>1 server</t>
-  </si>
-  <si>
     <t>550th - 196 ms</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
   </si>
   <si>
     <t>370th - 89 ms</t>
-  </si>
-  <si>
-    <t>2 servers</t>
   </si>
   <si>
     <t>prime numbers unix time</t>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>Ping AlgServer2 -&gt; Web</t>
+  </si>
+  <si>
+    <t>Jeden server</t>
+  </si>
+  <si>
+    <t>Dva servery</t>
   </si>
 </sst>
 </file>
@@ -311,13 +311,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -345,6 +342,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,6 +366,2239 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RPS!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jeden server</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RPS!$C$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RPS!$C$33:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16.326000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7939999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8239999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CEC0-4310-8045-378C5A3997F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RPS!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dva servery</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RPS!$G$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RPS!$G$33:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32.143999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.240000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7119999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CEC0-4310-8045-378C5A3997F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="351043576"/>
+        <c:axId val="351042264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="351043576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Průměrná délka spuštění algoritmu pro výpočet n-tého prvočísla [ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351042264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="351042264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Průměrný počet dotazů za sekundu</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351043576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RPS!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jeden server</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RPS!$C$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RPS!$C$34:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.2739999999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D3B-44F9-AA00-885C67BC7C01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RPS!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dva servery</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RPS!$G$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RPS!$G$34:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.98165800000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0280000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4259999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0D3B-44F9-AA00-885C67BC7C01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="351043576"/>
+        <c:axId val="351042264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="351043576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Průměrná délka spuštění algoritmu pro výpočet n-tého prvočísla [ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351042264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="351042264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Průměrná</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>rychlost odezvy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351043576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{734AF37F-822B-4264-AA35-CDAFF3DB362A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>338138</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3F2726C-EA95-494C-9769-E8BF3D529034}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1922,8 +4161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +4206,7 @@
         <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
         <v>13</v>
@@ -2790,11 +5029,11 @@
       <c r="E30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <f>_xlfn.STDEV.P(F4:F27)</f>
         <v>6.1585914560248787</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <f>_xlfn.STDEV.P(G4:G27)</f>
         <v>6.0718238816684842</v>
       </c>
@@ -2846,11 +5085,11 @@
         <v>420</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" ref="F34:F56" si="4">C34-D34</f>
+        <f t="shared" ref="F34:F55" si="4">C34-D34</f>
         <v>296.70799999999997</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" ref="G34:G56" si="5">E34-D34</f>
+        <f t="shared" ref="G34:G55" si="5">E34-D34</f>
         <v>309.00799999999998</v>
       </c>
       <c r="H34" t="b">
@@ -3351,12 +5590,32 @@
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" s="2">
+        <f>AVERAGE(F33:F55)</f>
+        <v>224.01021739130428</v>
+      </c>
+      <c r="G57" s="2">
+        <f>AVERAGE(G33:G55)</f>
+        <v>235.12326086956523</v>
+      </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" s="2">
+        <f>_xlfn.STDEV.P(F33:F55)</f>
+        <v>36.869620873932881</v>
+      </c>
+      <c r="G58" s="2">
+        <f>_xlfn.STDEV.P(G33:G55)</f>
+        <v>37.898348280191897</v>
+      </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C59" s="2"/>
@@ -3475,6 +5734,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -3482,8 +5742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:J10"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,21 +5757,21 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <v>645</v>
@@ -3522,779 +5782,805 @@
       <c r="E2">
         <v>16.55</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.82410000000000005</v>
       </c>
       <c r="G2">
         <v>120.56</v>
       </c>
     </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="21">
+        <v>89</v>
+      </c>
+      <c r="D5" s="21">
+        <v>196</v>
+      </c>
+      <c r="E5" s="21">
+        <v>492</v>
+      </c>
+      <c r="F5" s="21">
+        <v>985</v>
+      </c>
+      <c r="G5" s="21">
+        <v>89</v>
+      </c>
+      <c r="H5" s="21">
+        <v>196</v>
+      </c>
+      <c r="I5" s="21">
+        <v>492</v>
+      </c>
+      <c r="J5" s="22">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>16.36</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8.69</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3.82</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.86</v>
+      </c>
+      <c r="G6" s="4">
+        <v>33.33</v>
+      </c>
+      <c r="H6" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="I6" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="C7" s="6">
+        <v>1.89</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3.45</v>
+      </c>
+      <c r="E7" s="6">
+        <v>7.14</v>
+      </c>
+      <c r="F7" s="6">
+        <v>12.47</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.94445000000000001</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1.77</v>
+      </c>
+      <c r="I7" s="6">
+        <v>3.93</v>
+      </c>
+      <c r="J7" s="7">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="6">
+        <v>340.15</v>
+      </c>
+      <c r="D8" s="6">
+        <v>438.04</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F8" s="6">
+        <v>4620</v>
+      </c>
+      <c r="G8" s="6">
+        <v>138.97</v>
+      </c>
+      <c r="H8" s="6">
+        <v>200.63</v>
+      </c>
+      <c r="I8" s="6">
+        <v>686.24</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.83789999999999998</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.90480000000000005</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.8468</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.75929999999999997</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.74529999999999996</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.75939999999999996</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.85450000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="D10" s="8">
+        <v>4.71</v>
+      </c>
+      <c r="E10" s="8">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="F10" s="8">
+        <v>18.149999999999999</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1.85</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="I10" s="8">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="J10" s="9">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
-        <v>16.36</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8.69</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3.82</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="C11" s="4">
+        <v>15.85</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3.69</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="G11" s="4">
+        <v>31.58</v>
+      </c>
+      <c r="H11" s="4">
+        <v>17</v>
+      </c>
+      <c r="I11" s="4">
+        <v>7.38</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3.67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1.96</v>
+      </c>
+      <c r="D12" s="6">
+        <v>3.42</v>
+      </c>
+      <c r="E12" s="6">
+        <v>7.44</v>
+      </c>
+      <c r="F12" s="6">
+        <v>12.87</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.99858000000000002</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1.82</v>
+      </c>
+      <c r="I12" s="6">
+        <v>4.01</v>
+      </c>
+      <c r="J12" s="7">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="6">
+        <v>314.5</v>
+      </c>
+      <c r="D13" s="6">
+        <v>651.54</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1700</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6310</v>
+      </c>
+      <c r="G13" s="6">
+        <v>220.78</v>
+      </c>
+      <c r="H13" s="6">
+        <v>200.73</v>
+      </c>
+      <c r="I13" s="6">
+        <v>602.49</v>
+      </c>
+      <c r="J13" s="7">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.85060000000000002</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.90149999999999997</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.82879999999999998</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.54169999999999996</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.84519999999999995</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.77029999999999998</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.87849999999999995</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.81310000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3.07</v>
+      </c>
+      <c r="D15" s="8">
+        <v>4.26</v>
+      </c>
+      <c r="E15" s="8">
+        <v>9.61</v>
+      </c>
+      <c r="F15" s="8">
+        <v>22.33</v>
+      </c>
+      <c r="G15" s="8">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="H15" s="8">
+        <v>2.77</v>
+      </c>
+      <c r="I15" s="8">
+        <v>5.55</v>
+      </c>
+      <c r="J15" s="9">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>15.55</v>
+      </c>
+      <c r="D16" s="6">
+        <v>8.75</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3.79</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="G16" s="6">
+        <v>32.9</v>
+      </c>
+      <c r="H16" s="6">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="I16" s="6">
+        <v>7.39</v>
+      </c>
+      <c r="J16" s="7">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1.96</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3.42</v>
+      </c>
+      <c r="E17" s="6">
+        <v>7.39</v>
+      </c>
+      <c r="F17" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.95526</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="I17" s="6">
+        <v>4.03</v>
+      </c>
+      <c r="J17" s="7">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="6">
+        <v>268.07</v>
+      </c>
+      <c r="D18" s="6">
+        <v>397.58</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1720</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4920</v>
+      </c>
+      <c r="G18" s="6">
+        <v>152.33000000000001</v>
+      </c>
+      <c r="H18" s="6">
+        <v>203.23</v>
+      </c>
+      <c r="I18" s="6">
+        <v>565.24</v>
+      </c>
+      <c r="J18" s="7">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.77729999999999999</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.8821</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.84209999999999996</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.78949999999999998</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.77939999999999998</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.81579999999999997</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.88790000000000002</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0.85189999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2.92</v>
+      </c>
+      <c r="D20" s="6">
+        <v>4.53</v>
+      </c>
+      <c r="E20" s="6">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="F20" s="6">
+        <v>16.23</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="H20" s="6">
+        <v>2.38</v>
+      </c>
+      <c r="I20" s="6">
+        <v>5.45</v>
+      </c>
+      <c r="J20" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>16.91</v>
+      </c>
+      <c r="D21" s="4">
+        <v>8.41</v>
+      </c>
+      <c r="E21" s="4">
+        <v>3.77</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="G21" s="4">
+        <v>31.4</v>
+      </c>
+      <c r="H21" s="4">
+        <v>17.48</v>
+      </c>
+      <c r="I21" s="4">
+        <v>7.12</v>
+      </c>
+      <c r="J21" s="5">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1.82</v>
+      </c>
+      <c r="D22" s="6">
+        <v>3.58</v>
+      </c>
+      <c r="E22" s="6">
+        <v>7.26</v>
+      </c>
+      <c r="F22" s="6">
+        <v>12.15</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="I22" s="6">
+        <v>4.17</v>
+      </c>
+      <c r="J22" s="7">
+        <v>7.36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="6">
+        <v>199.17</v>
+      </c>
+      <c r="D23" s="6">
+        <v>557.13</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1950</v>
+      </c>
+      <c r="F23" s="6">
+        <v>4930</v>
+      </c>
+      <c r="G23" s="6">
+        <v>171.75</v>
+      </c>
+      <c r="H23" s="6">
+        <v>206.56</v>
+      </c>
+      <c r="I23" s="6">
+        <v>601.9</v>
+      </c>
+      <c r="J23" s="7">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.83460000000000001</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.88539999999999996</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.84350000000000003</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.78949999999999998</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.73819999999999997</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0.78459999999999996</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.82520000000000004</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0.83489999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2.54</v>
+      </c>
+      <c r="D25" s="8">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="E25" s="8">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F25" s="8">
+        <v>16.41</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1.91</v>
+      </c>
+      <c r="H25" s="8">
+        <v>2.64</v>
+      </c>
+      <c r="I25" s="8">
+        <v>6.13</v>
+      </c>
+      <c r="J25" s="9">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6">
+        <v>16.96</v>
+      </c>
+      <c r="D26" s="6">
+        <v>8.75</v>
+      </c>
+      <c r="E26" s="10">
+        <v>3.9</v>
+      </c>
+      <c r="F26" s="10">
         <v>1.86</v>
       </c>
-      <c r="G6" s="5">
-        <v>33.33</v>
-      </c>
-      <c r="H6" s="5">
-        <v>17.5</v>
-      </c>
-      <c r="I6" s="5">
-        <v>7.6</v>
-      </c>
-      <c r="J6" s="6">
-        <v>3.79</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="G26" s="6">
+        <v>31.51</v>
+      </c>
+      <c r="H26" s="6">
+        <v>16.78</v>
+      </c>
+      <c r="I26" s="6">
+        <v>7.43</v>
+      </c>
+      <c r="J26" s="7">
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1.82</v>
+      </c>
+      <c r="D27" s="6">
+        <v>3.45</v>
+      </c>
+      <c r="E27" s="10">
+        <v>7.14</v>
+      </c>
+      <c r="F27" s="10">
+        <v>12.4</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1.85</v>
+      </c>
+      <c r="I27" s="6">
+        <v>4</v>
+      </c>
+      <c r="J27" s="7">
+        <v>7.64</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="6">
+        <v>217.94</v>
+      </c>
+      <c r="D28" s="6">
+        <v>697.48</v>
+      </c>
+      <c r="E28" s="10">
+        <v>2020</v>
+      </c>
+      <c r="F28" s="10">
+        <v>4630</v>
+      </c>
+      <c r="G28" s="6">
+        <v>238.47</v>
+      </c>
+      <c r="H28" s="6">
+        <v>295.52</v>
+      </c>
+      <c r="I28" s="6">
+        <v>738.98</v>
+      </c>
+      <c r="J28" s="7">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7">
-        <v>1.89</v>
-      </c>
-      <c r="D7" s="7">
-        <v>3.45</v>
-      </c>
-      <c r="E7" s="7">
-        <v>7.14</v>
-      </c>
-      <c r="F7" s="7">
-        <v>12.47</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0.94445000000000001</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1.77</v>
-      </c>
-      <c r="I7" s="7">
-        <v>3.93</v>
-      </c>
-      <c r="J7" s="8">
-        <v>7.28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="C29" s="6">
+        <v>0.84750000000000003</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.84409999999999996</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0.76790000000000003</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.89219999999999999</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="I29" s="6">
+        <v>0.86040000000000005</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="7">
-        <v>340.15</v>
-      </c>
-      <c r="D8" s="7">
-        <v>438.04</v>
-      </c>
-      <c r="E8" s="7">
-        <v>2000</v>
-      </c>
-      <c r="F8" s="7">
-        <v>4620</v>
-      </c>
-      <c r="G8" s="7">
-        <v>138.97</v>
-      </c>
-      <c r="H8" s="7">
-        <v>200.63</v>
-      </c>
-      <c r="I8" s="7">
-        <v>686.24</v>
-      </c>
-      <c r="J8" s="8">
-        <v>1780</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0.83789999999999998</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.90480000000000005</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0.8468</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0.75929999999999997</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0.74529999999999996</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0.75939999999999996</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0.85450000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2.8</v>
-      </c>
-      <c r="D10" s="9">
-        <v>4.71</v>
-      </c>
-      <c r="E10" s="9">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="F10" s="9">
-        <v>18.149999999999999</v>
-      </c>
-      <c r="G10" s="9">
-        <v>1.85</v>
-      </c>
-      <c r="H10" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="I10" s="9">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="J10" s="10">
-        <v>8.76</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5">
-        <v>15.85</v>
-      </c>
-      <c r="D11" s="5">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E11" s="5">
-        <v>3.69</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="G11" s="5">
-        <v>31.58</v>
-      </c>
-      <c r="H11" s="5">
-        <v>17</v>
-      </c>
-      <c r="I11" s="5">
-        <v>7.38</v>
-      </c>
-      <c r="J11" s="6">
-        <v>3.67</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1.96</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3.42</v>
-      </c>
-      <c r="E12" s="7">
-        <v>7.44</v>
-      </c>
-      <c r="F12" s="7">
-        <v>12.87</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0.99858000000000002</v>
-      </c>
-      <c r="H12" s="7">
-        <v>1.82</v>
-      </c>
-      <c r="I12" s="7">
-        <v>4.01</v>
-      </c>
-      <c r="J12" s="8">
-        <v>7.47</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="7">
-        <v>314.5</v>
-      </c>
-      <c r="D13" s="7">
-        <v>651.54</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1700</v>
-      </c>
-      <c r="F13" s="7">
-        <v>6310</v>
-      </c>
-      <c r="G13" s="7">
-        <v>220.78</v>
-      </c>
-      <c r="H13" s="7">
-        <v>200.73</v>
-      </c>
-      <c r="I13" s="7">
-        <v>602.49</v>
-      </c>
-      <c r="J13" s="8">
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="7">
-        <v>0.85060000000000002</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0.90149999999999997</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0.82879999999999998</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0.54169999999999996</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0.84519999999999995</v>
-      </c>
-      <c r="H14" s="7">
-        <v>0.77029999999999998</v>
-      </c>
-      <c r="I14" s="7">
-        <v>0.87849999999999995</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0.81310000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="9">
-        <v>3.07</v>
-      </c>
-      <c r="D15" s="9">
-        <v>4.26</v>
-      </c>
-      <c r="E15" s="9">
-        <v>9.61</v>
-      </c>
-      <c r="F15" s="9">
-        <v>22.33</v>
-      </c>
-      <c r="G15" s="9">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="H15" s="9">
-        <v>2.77</v>
-      </c>
-      <c r="I15" s="9">
-        <v>5.55</v>
-      </c>
-      <c r="J15" s="10">
-        <v>9.68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7">
-        <v>15.55</v>
-      </c>
-      <c r="D16" s="7">
-        <v>8.75</v>
-      </c>
-      <c r="E16" s="7">
-        <v>3.79</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1.9</v>
-      </c>
-      <c r="G16" s="7">
-        <v>32.9</v>
-      </c>
-      <c r="H16" s="7">
-        <v>17.440000000000001</v>
-      </c>
-      <c r="I16" s="7">
-        <v>7.39</v>
-      </c>
-      <c r="J16" s="8">
-        <v>3.73</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1.96</v>
-      </c>
-      <c r="D17" s="7">
-        <v>3.42</v>
-      </c>
-      <c r="E17" s="7">
-        <v>7.39</v>
-      </c>
-      <c r="F17" s="7">
-        <v>12.1</v>
-      </c>
-      <c r="G17" s="7">
-        <v>0.95526</v>
-      </c>
-      <c r="H17" s="7">
-        <v>1.78</v>
-      </c>
-      <c r="I17" s="7">
-        <v>4.03</v>
-      </c>
-      <c r="J17" s="8">
-        <v>7.38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="7">
-        <v>268.07</v>
-      </c>
-      <c r="D18" s="7">
-        <v>397.58</v>
-      </c>
-      <c r="E18" s="7">
-        <v>1720</v>
-      </c>
-      <c r="F18" s="7">
-        <v>4920</v>
-      </c>
-      <c r="G18" s="7">
-        <v>152.33000000000001</v>
-      </c>
-      <c r="H18" s="7">
-        <v>203.23</v>
-      </c>
-      <c r="I18" s="7">
-        <v>565.24</v>
-      </c>
-      <c r="J18" s="8">
-        <v>1820</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="7">
-        <v>0.77729999999999999</v>
-      </c>
-      <c r="D19" s="7">
-        <v>0.8821</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0.84209999999999996</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0.78949999999999998</v>
-      </c>
-      <c r="G19" s="7">
-        <v>0.77939999999999998</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0.81579999999999997</v>
-      </c>
-      <c r="I19" s="7">
-        <v>0.88790000000000002</v>
-      </c>
-      <c r="J19" s="8">
-        <v>0.85189999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="C30" s="8">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="D30" s="8">
+        <v>4.49</v>
+      </c>
+      <c r="E30" s="8">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F30" s="8">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="G30" s="8">
+        <v>2.63</v>
+      </c>
+      <c r="H30" s="8">
         <v>2.92</v>
       </c>
-      <c r="D20" s="7">
-        <v>4.53</v>
-      </c>
-      <c r="E20" s="7">
-        <v>9.5299999999999994</v>
-      </c>
-      <c r="F20" s="7">
-        <v>16.23</v>
-      </c>
-      <c r="G20" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="H20" s="7">
-        <v>2.38</v>
-      </c>
-      <c r="I20" s="7">
-        <v>5.45</v>
-      </c>
-      <c r="J20" s="8">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5">
-        <v>16.91</v>
-      </c>
-      <c r="D21" s="5">
-        <v>8.41</v>
-      </c>
-      <c r="E21" s="5">
-        <v>3.77</v>
-      </c>
-      <c r="F21" s="5">
-        <v>1.9</v>
-      </c>
-      <c r="G21" s="5">
-        <v>31.4</v>
-      </c>
-      <c r="H21" s="5">
-        <v>17.48</v>
-      </c>
-      <c r="I21" s="5">
-        <v>7.12</v>
-      </c>
-      <c r="J21" s="6">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="7">
-        <v>1.82</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3.58</v>
-      </c>
-      <c r="E22" s="7">
-        <v>7.26</v>
-      </c>
-      <c r="F22" s="7">
-        <v>12.15</v>
-      </c>
-      <c r="G22" s="7">
-        <v>1</v>
-      </c>
-      <c r="H22" s="7">
-        <v>1.78</v>
-      </c>
-      <c r="I22" s="7">
-        <v>4.17</v>
-      </c>
-      <c r="J22" s="8">
-        <v>7.36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="7">
-        <v>199.17</v>
-      </c>
-      <c r="D23" s="7">
-        <v>557.13</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1950</v>
-      </c>
-      <c r="F23" s="7">
-        <v>4930</v>
-      </c>
-      <c r="G23" s="7">
-        <v>171.75</v>
-      </c>
-      <c r="H23" s="7">
-        <v>206.56</v>
-      </c>
-      <c r="I23" s="7">
-        <v>601.9</v>
-      </c>
-      <c r="J23" s="8">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0.83460000000000001</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0.88539999999999996</v>
-      </c>
-      <c r="E24" s="7">
-        <v>0.84350000000000003</v>
-      </c>
-      <c r="F24" s="7">
-        <v>0.78949999999999998</v>
-      </c>
-      <c r="G24" s="7">
-        <v>0.73819999999999997</v>
-      </c>
-      <c r="H24" s="7">
-        <v>0.78459999999999996</v>
-      </c>
-      <c r="I24" s="7">
-        <v>0.82520000000000004</v>
-      </c>
-      <c r="J24" s="8">
-        <v>0.83489999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="9">
-        <v>2.54</v>
-      </c>
-      <c r="D25" s="9">
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="E25" s="9">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="F25" s="9">
-        <v>16.41</v>
-      </c>
-      <c r="G25" s="9">
-        <v>1.91</v>
-      </c>
-      <c r="H25" s="9">
-        <v>2.64</v>
-      </c>
-      <c r="I25" s="9">
-        <v>6.13</v>
-      </c>
-      <c r="J25" s="10">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7">
-        <v>16.96</v>
-      </c>
-      <c r="D26" s="7">
-        <v>8.75</v>
-      </c>
-      <c r="E26" s="11">
-        <v>3.9</v>
-      </c>
-      <c r="F26" s="11">
-        <v>1.86</v>
-      </c>
-      <c r="G26" s="7">
-        <v>31.51</v>
-      </c>
-      <c r="H26" s="7">
-        <v>16.78</v>
-      </c>
-      <c r="I26" s="7">
-        <v>7.43</v>
-      </c>
-      <c r="J26" s="8">
-        <v>3.62</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="7">
-        <v>1.82</v>
-      </c>
-      <c r="D27" s="7">
-        <v>3.45</v>
-      </c>
-      <c r="E27" s="11">
-        <v>7.14</v>
-      </c>
-      <c r="F27" s="11">
-        <v>12.4</v>
-      </c>
-      <c r="G27" s="7">
-        <v>1.01</v>
-      </c>
-      <c r="H27" s="7">
-        <v>1.85</v>
-      </c>
-      <c r="I27" s="7">
-        <v>4</v>
-      </c>
-      <c r="J27" s="8">
-        <v>7.64</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="7">
-        <v>217.94</v>
-      </c>
-      <c r="D28" s="7">
-        <v>697.48</v>
-      </c>
-      <c r="E28" s="11">
-        <v>2020</v>
-      </c>
-      <c r="F28" s="11">
-        <v>4630</v>
-      </c>
-      <c r="G28" s="7">
-        <v>238.47</v>
-      </c>
-      <c r="H28" s="7">
-        <v>295.52</v>
-      </c>
-      <c r="I28" s="7">
-        <v>738.98</v>
-      </c>
-      <c r="J28" s="8">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0.84750000000000003</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0.84409999999999996</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0.84619999999999995</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0.76790000000000003</v>
-      </c>
-      <c r="G29" s="7">
-        <v>0.89219999999999999</v>
-      </c>
-      <c r="H29" s="7">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="I29" s="7">
-        <v>0.86040000000000005</v>
-      </c>
-      <c r="J29" s="8">
-        <v>0.78900000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="9">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="D30" s="9">
-        <v>4.49</v>
-      </c>
-      <c r="E30" s="9">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="F30" s="9">
-        <v>17.649999999999999</v>
-      </c>
-      <c r="G30" s="9">
-        <v>2.63</v>
-      </c>
-      <c r="H30" s="9">
-        <v>2.92</v>
-      </c>
-      <c r="I30" s="9">
+      <c r="I30" s="8">
         <v>5.41</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="9">
         <v>9.3800000000000008</v>
       </c>
     </row>
@@ -4304,7 +6590,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C33">
@@ -4341,8 +6627,8 @@
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
-        <v>26</v>
+      <c r="B34" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="C34">
         <f>AVERAGE(C27,C22,C17,C12,C7)</f>
@@ -4378,8 +6664,8 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
-        <v>27</v>
+      <c r="B35" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="C35">
         <f>AVERAGE(C28,C23,C18,C13,C8)</f>
@@ -4415,45 +6701,45 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="4">
-        <f t="shared" ref="C34:J37" si="3">AVERAGE(C29,C24,C19,C14,C9)</f>
+      <c r="B36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" ref="C36:J37" si="3">AVERAGE(C29,C24,C19,C14,C9)</f>
         <v>0.82957999999999998</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <f t="shared" si="3"/>
         <v>0.88357999999999992</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <f t="shared" si="3"/>
         <v>0.84148000000000001</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="3">
         <f t="shared" si="3"/>
         <v>0.72958000000000001</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <f t="shared" si="3"/>
         <v>0.80005999999999999</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <f t="shared" si="3"/>
         <v>0.79261999999999988</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="3">
         <f t="shared" si="3"/>
         <v>0.87319999999999998</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="3">
         <f t="shared" si="3"/>
         <v>0.82867999999999997</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
-        <v>29</v>
+      <c r="B37" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="C37">
         <f t="shared" si="3"/>
@@ -4489,16 +6775,16 @@
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C122" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
+      <c r="C122" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D122" s="20"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="20"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C123">
         <v>370</v>
@@ -4734,19 +7020,20 @@
     <mergeCell ref="C122:F122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="C138:F138" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4757,221 +7044,286 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>36</v>
+      <c r="C2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>6.82</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>6.4</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3.41</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="D5" s="8">
-        <v>4.6100000000000003</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="C7" s="6">
+        <v>0.62039999999999995</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7">
-        <v>3.41</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="7">
-        <v>0.62039999999999995</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.77080000000000004</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>14.58</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>8.8800000000000008</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>6.63</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>7.02</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4.09</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3.18</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7">
-        <v>4.09</v>
-      </c>
-      <c r="D10" s="8">
+      <c r="C12" s="6">
+        <v>0.54769999999999996</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.72989999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="8">
+        <v>9.19</v>
+      </c>
+      <c r="D13" s="9">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>6.92</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6">
+        <v>4.18</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3.66</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.61060000000000003</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.69379999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="8">
+        <v>9.16</v>
+      </c>
+      <c r="D18" s="9">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f>AVERAGE(C4,C9,C14)</f>
+        <v>6.7899999999999991</v>
+      </c>
+      <c r="D20">
+        <f>AVERAGE(D4,D9,D14)</f>
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:D24" si="0">AVERAGE(C5,C10,C15)</f>
         <v>4.21</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>4.3366666666666669</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>3.4166666666666665</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1.1366666666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.59289999999999998</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.73150000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7">
-        <v>3.18</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="7">
-        <v>0.54769999999999996</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.72989999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="9">
-        <v>9.19</v>
-      </c>
-      <c r="D13" s="10">
-        <v>6.16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="5">
-        <v>6.92</v>
-      </c>
-      <c r="D14" s="6">
-        <v>6.95</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="7">
-        <v>4.18</v>
-      </c>
-      <c r="D15" s="8">
-        <v>4.1900000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3.66</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0.61060000000000003</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0.69379999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="9">
-        <v>9.16</v>
-      </c>
-      <c r="D18" s="10">
-        <v>6.1</v>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>10.976666666666667</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>7.0466666666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>